<commit_message>
Fixed several additional calculations, established 1/SE as the new measure of precision
</commit_message>
<xml_diff>
--- a/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
+++ b/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Tools and meta-analysis theory\Delta method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C0D73F-59C8-4FA7-94BF-B62F9DFD4125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D4FD15-EDA3-4FE6-9411-565D531927D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -641,8 +641,8 @@
   <dimension ref="A1:G580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D565" sqref="D565"/>
+      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C304" sqref="C304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7378,7 +7378,7 @@
         <v>1</v>
       </c>
       <c r="C293" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D293">
         <v>8.7999999999999995E-2</v>
@@ -7401,7 +7401,7 @@
         <v>1</v>
       </c>
       <c r="C294" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D294">
         <v>0.126</v>
@@ -7424,7 +7424,7 @@
         <v>1</v>
       </c>
       <c r="C295" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D295">
         <v>7.0999999999999994E-2</v>
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="C296" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D296">
         <v>8.9999999999999993E-3</v>
@@ -7470,7 +7470,7 @@
         <v>1</v>
       </c>
       <c r="C297" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D297">
         <v>9.2999999999999999E-2</v>
@@ -7493,7 +7493,7 @@
         <v>1</v>
       </c>
       <c r="C298" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D298">
         <v>-1.0999999999999999E-2</v>
@@ -7516,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="C299" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D299">
         <v>8.5000000000000006E-2</v>
@@ -7539,7 +7539,7 @@
         <v>1</v>
       </c>
       <c r="C300" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D300">
         <v>-9.0999999999999998E-2</v>
@@ -7562,7 +7562,7 @@
         <v>1</v>
       </c>
       <c r="C301" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D301">
         <v>5.1999999999999998E-2</v>
@@ -7585,7 +7585,7 @@
         <v>1</v>
       </c>
       <c r="C302" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D302">
         <v>0.222</v>
@@ -7608,7 +7608,7 @@
         <v>1</v>
       </c>
       <c r="C303" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D303">
         <v>3.6999999999999998E-2</v>
@@ -7631,7 +7631,7 @@
         <v>1</v>
       </c>
       <c r="C304" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D304">
         <v>0.23</v>
@@ -7654,14 +7654,13 @@
         <v>1</v>
       </c>
       <c r="C305" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D305">
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="E305">
-        <f>D305/100</f>
-        <v>9.68E-4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F305">
         <v>999</v>
@@ -7675,24 +7674,22 @@
         <v>27</v>
       </c>
       <c r="B306" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C306" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D306">
         <v>0.13699999999999998</v>
       </c>
       <c r="E306">
-        <f t="shared" ref="E306:G325" si="0">D306/100</f>
-        <v>1.3699999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F306">
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="G306">
-        <f>F306/100</f>
-        <v>9.68E-4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -7700,24 +7697,22 @@
         <v>27</v>
       </c>
       <c r="B307" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C307" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D307">
         <v>0.26899999999999996</v>
       </c>
       <c r="E307">
-        <f t="shared" si="0"/>
-        <v>2.6899999999999997E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F307">
-        <v>0.13699999999999998</v>
+        <v>9.6799999999999997E-2</v>
       </c>
       <c r="G307">
-        <f t="shared" si="0"/>
-        <v>1.3699999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
@@ -7728,21 +7723,19 @@
         <v>1</v>
       </c>
       <c r="C308" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D308">
         <v>0.10300000000000001</v>
       </c>
       <c r="E308">
-        <f t="shared" si="0"/>
-        <v>1.0300000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F308">
         <v>0.26899999999999996</v>
       </c>
       <c r="G308">
-        <f t="shared" si="0"/>
-        <v>2.6899999999999997E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -7750,24 +7743,22 @@
         <v>27</v>
       </c>
       <c r="B309" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C309" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D309">
         <v>0.14499999999999999</v>
       </c>
       <c r="E309">
-        <f t="shared" si="0"/>
-        <v>1.4499999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F309">
         <v>0.10300000000000001</v>
       </c>
       <c r="G309">
-        <f t="shared" si="0"/>
-        <v>1.0300000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
@@ -7775,24 +7766,22 @@
         <v>27</v>
       </c>
       <c r="B310" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C310" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D310">
         <v>0.28399999999999997</v>
       </c>
       <c r="E310">
-        <f t="shared" si="0"/>
-        <v>2.8399999999999996E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F310">
-        <v>0.14499999999999999</v>
+        <v>0.10300000000000001</v>
       </c>
       <c r="G310">
-        <f t="shared" si="0"/>
-        <v>1.4499999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
@@ -7803,21 +7792,19 @@
         <v>1</v>
       </c>
       <c r="C311" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D311">
         <v>9.9399999999999988E-2</v>
       </c>
       <c r="E311">
-        <f t="shared" si="0"/>
-        <v>9.9399999999999987E-4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F311">
         <v>0.28399999999999997</v>
       </c>
       <c r="G311">
-        <f t="shared" si="0"/>
-        <v>2.8399999999999996E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -7825,24 +7812,22 @@
         <v>27</v>
       </c>
       <c r="B312" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C312" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D312">
         <v>0.13900000000000001</v>
       </c>
       <c r="E312">
-        <f t="shared" si="0"/>
-        <v>1.3900000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F312">
         <v>9.9399999999999988E-2</v>
       </c>
       <c r="G312">
-        <f t="shared" si="0"/>
-        <v>9.9399999999999987E-4</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
@@ -7850,24 +7835,22 @@
         <v>27</v>
       </c>
       <c r="B313" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C313" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D313">
         <v>0.27699999999999997</v>
       </c>
       <c r="E313">
-        <f t="shared" si="0"/>
-        <v>2.7699999999999999E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F313">
-        <v>0.13900000000000001</v>
+        <v>9.9399999999999988E-2</v>
       </c>
       <c r="G313">
-        <f t="shared" si="0"/>
-        <v>1.3900000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
@@ -7878,21 +7861,19 @@
         <v>1</v>
       </c>
       <c r="C314" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D314">
         <v>5.5E-2</v>
       </c>
       <c r="E314">
-        <f t="shared" si="0"/>
-        <v>5.5000000000000003E-4</v>
+        <v>0.01</v>
       </c>
       <c r="F314">
         <v>0.27699999999999997</v>
       </c>
       <c r="G314">
-        <f t="shared" si="0"/>
-        <v>2.7699999999999999E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
@@ -7900,24 +7881,22 @@
         <v>27</v>
       </c>
       <c r="B315" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C315" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D315">
         <v>0.11</v>
       </c>
       <c r="E315">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F315">
         <v>5.5E-2</v>
       </c>
       <c r="G315">
-        <f t="shared" si="0"/>
-        <v>5.5000000000000003E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
@@ -7925,24 +7904,22 @@
         <v>27</v>
       </c>
       <c r="B316" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C316" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D316">
         <v>0.21899999999999997</v>
       </c>
       <c r="E316">
-        <f t="shared" si="0"/>
-        <v>2.1899999999999997E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F316">
-        <v>0.11</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G316">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
@@ -7953,21 +7930,19 @@
         <v>1</v>
       </c>
       <c r="C317" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D317">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="E317">
-        <f t="shared" si="0"/>
-        <v>6.0999999999999997E-4</v>
+        <v>0.01</v>
       </c>
       <c r="F317">
         <v>0.21899999999999997</v>
       </c>
       <c r="G317">
-        <f t="shared" si="0"/>
-        <v>2.1899999999999997E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
@@ -7975,24 +7950,22 @@
         <v>27</v>
       </c>
       <c r="B318" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C318" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D318">
         <v>0.122</v>
       </c>
       <c r="E318">
-        <f t="shared" si="0"/>
-        <v>1.2199999999999999E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F318">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="G318">
-        <f t="shared" si="0"/>
-        <v>6.0999999999999997E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
@@ -8000,24 +7973,22 @@
         <v>27</v>
       </c>
       <c r="B319" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C319" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D319">
         <v>0.24600000000000002</v>
       </c>
       <c r="E319">
-        <f t="shared" si="0"/>
-        <v>2.4600000000000004E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F319">
-        <v>0.122</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="G319">
-        <f t="shared" si="0"/>
-        <v>1.2199999999999999E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
@@ -8028,21 +7999,19 @@
         <v>1</v>
       </c>
       <c r="C320" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D320">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E320">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000001E-4</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="F320">
         <v>0.24600000000000002</v>
       </c>
       <c r="G320">
-        <f t="shared" si="0"/>
-        <v>2.4600000000000004E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
@@ -8050,24 +8019,22 @@
         <v>27</v>
       </c>
       <c r="B321" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C321" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D321">
         <v>0.10800000000000001</v>
       </c>
       <c r="E321">
-        <f t="shared" si="0"/>
-        <v>1.0800000000000002E-3</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="F321">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="G321">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000001E-4</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -8075,24 +8042,22 @@
         <v>27</v>
       </c>
       <c r="B322" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C322" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D322">
         <v>0.22399999999999998</v>
       </c>
       <c r="E322">
-        <f t="shared" si="0"/>
-        <v>2.2399999999999998E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F322">
-        <v>0.10800000000000001</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G322">
-        <f t="shared" si="0"/>
-        <v>1.0800000000000002E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
@@ -8103,21 +8068,19 @@
         <v>1</v>
       </c>
       <c r="C323" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D323">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E323">
-        <f t="shared" si="0"/>
-        <v>5.2999999999999998E-4</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="F323">
         <v>0.22399999999999998</v>
       </c>
       <c r="G323">
-        <f t="shared" si="0"/>
-        <v>2.2399999999999998E-3</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
@@ -8125,24 +8088,22 @@
         <v>27</v>
       </c>
       <c r="B324" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C324" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D324">
         <v>0.12</v>
       </c>
       <c r="E324">
-        <f t="shared" si="0"/>
-        <v>1.1999999999999999E-3</v>
+        <v>1.3000000000000001E-2</v>
       </c>
       <c r="F324">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="G324">
-        <f t="shared" si="0"/>
-        <v>5.2999999999999998E-4</v>
+        <v>1.1000000000000001E-2</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.25">
@@ -8150,24 +8111,22 @@
         <v>27</v>
       </c>
       <c r="B325" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C325" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D325">
         <v>0.22600000000000001</v>
       </c>
       <c r="E325">
-        <f t="shared" si="0"/>
-        <v>2.2599999999999999E-3</v>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="F325">
-        <v>0.12</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G325">
-        <f t="shared" si="0"/>
-        <v>1.1999999999999999E-3</v>
+        <v>1.1000000000000001E-2</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed incorrect data calculation for Kijima (2006). IV now works.
</commit_message>
<xml_diff>
--- a/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
+++ b/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Tools and meta-analysis theory\Delta method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D4FD15-EDA3-4FE6-9411-565D531927D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034EC26-2460-40DD-ADFA-BF6433C16113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,8 +641,8 @@
   <dimension ref="A1:G580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C304" sqref="C304"/>
+      <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H538" sqref="H538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12950,7 +12950,7 @@
         <v>0.161</v>
       </c>
       <c r="E535">
-        <v>3.41</v>
+        <v>4.7214076246334308E-2</v>
       </c>
       <c r="F535">
         <v>999</v>
@@ -12973,13 +12973,13 @@
         <v>0.47599999999999998</v>
       </c>
       <c r="E536">
-        <v>9.76</v>
+        <v>4.8770491803278686E-2</v>
       </c>
       <c r="F536">
         <v>0.161</v>
       </c>
       <c r="G536">
-        <v>3.41</v>
+        <v>4.7214076246334308E-2</v>
       </c>
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.25">
@@ -12996,13 +12996,13 @@
         <v>0.88100000000000001</v>
       </c>
       <c r="E537">
-        <v>15.59</v>
+        <v>5.6510583707504815E-2</v>
       </c>
       <c r="F537">
         <v>0.47599999999999998</v>
       </c>
       <c r="G537">
-        <v>9.76</v>
+        <v>4.8770491803278686E-2</v>
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.25">
@@ -13019,13 +13019,13 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="E538">
-        <v>2.2599999999999998</v>
+        <v>5.9292035398230095E-2</v>
       </c>
       <c r="F538">
         <v>0.88100000000000001</v>
       </c>
       <c r="G538">
-        <v>15.59</v>
+        <v>5.6510583707504815E-2</v>
       </c>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
@@ -13042,13 +13042,13 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="E539">
-        <v>8.1</v>
+        <v>5.4814814814814816E-2</v>
       </c>
       <c r="F539">
         <v>0.13400000000000001</v>
       </c>
       <c r="G539">
-        <v>2.2599999999999998</v>
+        <v>5.9292035398230095E-2</v>
       </c>
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
@@ -13065,13 +13065,13 @@
         <v>1.0129999999999999</v>
       </c>
       <c r="E540">
-        <v>17.3</v>
+        <v>5.8554913294797679E-2</v>
       </c>
       <c r="F540">
         <v>0.44400000000000001</v>
       </c>
       <c r="G540">
-        <v>8.1</v>
+        <v>5.4814814814814816E-2</v>
       </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
@@ -13088,13 +13088,13 @@
         <v>0.152</v>
       </c>
       <c r="E541">
-        <v>3.46</v>
+        <v>4.3930635838150288E-2</v>
       </c>
       <c r="F541">
         <v>1.0129999999999999</v>
       </c>
       <c r="G541">
-        <v>17.3</v>
+        <v>5.8554913294797679E-2</v>
       </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
@@ -13111,13 +13111,13 @@
         <v>0.438</v>
       </c>
       <c r="E542">
-        <v>9.27</v>
+        <v>4.7249190938511328E-2</v>
       </c>
       <c r="F542">
         <v>0.152</v>
       </c>
       <c r="G542">
-        <v>3.46</v>
+        <v>4.3930635838150288E-2</v>
       </c>
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
@@ -13134,13 +13134,13 @@
         <v>0.84</v>
       </c>
       <c r="E543">
-        <v>16.420000000000002</v>
+        <v>5.1157125456760044E-2</v>
       </c>
       <c r="F543">
         <v>0.438</v>
       </c>
       <c r="G543">
-        <v>9.27</v>
+        <v>4.7249190938511328E-2</v>
       </c>
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
@@ -13157,13 +13157,13 @@
         <v>0.17799999999999999</v>
       </c>
       <c r="E544">
-        <v>3.22</v>
+        <v>5.5279503105590058E-2</v>
       </c>
       <c r="F544">
         <v>0.84</v>
       </c>
       <c r="G544">
-        <v>16.420000000000002</v>
+        <v>5.1157125456760044E-2</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
@@ -13180,13 +13180,13 @@
         <v>0.45600000000000002</v>
       </c>
       <c r="E545">
-        <v>8.93</v>
+        <v>5.1063829787234047E-2</v>
       </c>
       <c r="F545">
         <v>0.17799999999999999</v>
       </c>
       <c r="G545">
-        <v>3.22</v>
+        <v>5.5279503105590058E-2</v>
       </c>
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
@@ -13203,13 +13203,13 @@
         <v>0.89600000000000002</v>
       </c>
       <c r="E546">
-        <v>16.649999999999999</v>
+        <v>5.3813813813813817E-2</v>
       </c>
       <c r="F546">
         <v>0.45600000000000002</v>
       </c>
       <c r="G546">
-        <v>8.93</v>
+        <v>5.1063829787234047E-2</v>
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
@@ -13226,13 +13226,13 @@
         <v>0.17799999999999999</v>
       </c>
       <c r="E547">
-        <v>3.58</v>
+        <v>4.9720670391061449E-2</v>
       </c>
       <c r="F547">
         <v>0.89600000000000002</v>
       </c>
       <c r="G547">
-        <v>16.649999999999999</v>
+        <v>5.3813813813813817E-2</v>
       </c>
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.25">
@@ -13249,13 +13249,13 @@
         <v>0.439</v>
       </c>
       <c r="E548">
-        <v>6.3</v>
+        <v>6.9682539682539679E-2</v>
       </c>
       <c r="F548">
         <v>0.17799999999999999</v>
       </c>
       <c r="G548">
-        <v>3.58</v>
+        <v>4.9720670391061449E-2</v>
       </c>
     </row>
     <row r="549" spans="1:7" x14ac:dyDescent="0.25">
@@ -13272,13 +13272,13 @@
         <v>0.81699999999999995</v>
       </c>
       <c r="E549">
-        <v>12.02</v>
+        <v>6.7970049916805317E-2</v>
       </c>
       <c r="F549">
         <v>0.439</v>
       </c>
       <c r="G549">
-        <v>6.3</v>
+        <v>6.9682539682539679E-2</v>
       </c>
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.25">
@@ -13295,13 +13295,13 @@
         <v>0.2</v>
       </c>
       <c r="E550">
-        <v>3.37</v>
+        <v>5.9347181008902079E-2</v>
       </c>
       <c r="F550">
         <v>0.81699999999999995</v>
       </c>
       <c r="G550">
-        <v>12.02</v>
+        <v>6.7970049916805317E-2</v>
       </c>
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.25">
@@ -13318,13 +13318,13 @@
         <v>0.53300000000000003</v>
       </c>
       <c r="E551">
-        <v>8.85</v>
+        <v>6.0225988700564975E-2</v>
       </c>
       <c r="F551">
         <v>0.2</v>
       </c>
       <c r="G551">
-        <v>3.37</v>
+        <v>5.9347181008902079E-2</v>
       </c>
     </row>
     <row r="552" spans="1:7" x14ac:dyDescent="0.25">
@@ -13341,13 +13341,13 @@
         <v>0.94699999999999995</v>
       </c>
       <c r="E552">
-        <v>12.3</v>
+        <v>7.6991869918699177E-2</v>
       </c>
       <c r="F552">
         <v>0.53300000000000003</v>
       </c>
       <c r="G552">
-        <v>8.85</v>
+        <v>6.0225988700564975E-2</v>
       </c>
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.25">
@@ -13364,13 +13364,13 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="E553">
-        <v>4.88</v>
+        <v>4.6516393442622955E-2</v>
       </c>
       <c r="F553">
         <v>0.94699999999999995</v>
       </c>
       <c r="G553">
-        <v>12.3</v>
+        <v>7.6991869918699177E-2</v>
       </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.25">
@@ -13387,13 +13387,13 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="E554">
-        <v>12.01</v>
+        <v>4.7210657785179015E-2</v>
       </c>
       <c r="F554">
         <v>0.22700000000000001</v>
       </c>
       <c r="G554">
-        <v>4.88</v>
+        <v>4.6516393442622955E-2</v>
       </c>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
@@ -13410,13 +13410,13 @@
         <v>0.79700000000000004</v>
       </c>
       <c r="E555">
-        <v>9.39</v>
+        <v>8.4877529286474976E-2</v>
       </c>
       <c r="F555">
         <v>0.56699999999999995</v>
       </c>
       <c r="G555">
-        <v>12.01</v>
+        <v>4.7210657785179015E-2</v>
       </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
@@ -13433,13 +13433,13 @@
         <v>0.221</v>
       </c>
       <c r="E556">
-        <v>3.36</v>
+        <v>6.5773809523809526E-2</v>
       </c>
       <c r="F556">
         <v>0.79700000000000004</v>
       </c>
       <c r="G556">
-        <v>9.39</v>
+        <v>8.4877529286474976E-2</v>
       </c>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
@@ -13456,13 +13456,13 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="E557">
-        <v>9.61</v>
+        <v>5.9729448491155045E-2</v>
       </c>
       <c r="F557">
         <v>0.221</v>
       </c>
       <c r="G557">
-        <v>3.36</v>
+        <v>6.5773809523809526E-2</v>
       </c>
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
@@ -13479,13 +13479,13 @@
         <v>1.0369999999999999</v>
       </c>
       <c r="E558">
-        <v>16.190000000000001</v>
+        <v>6.4051883878937607E-2</v>
       </c>
       <c r="F558">
         <v>0.57399999999999995</v>
       </c>
       <c r="G558">
-        <v>9.61</v>
+        <v>5.9729448491155045E-2</v>
       </c>
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed calculation for more studies
</commit_message>
<xml_diff>
--- a/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
+++ b/Tools and meta-analysis theory/Delta method/deltamethod_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Tools and meta-analysis theory\Delta method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034EC26-2460-40DD-ADFA-BF6433C16113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E80AB-CC40-4DFA-B67C-D096917E93ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -356,6 +356,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -641,8 +644,8 @@
   <dimension ref="A1:G580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H538" sqref="H538"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K162" sqref="K162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4224,10 +4227,10 @@
         <v>18</v>
       </c>
       <c r="B156" s="3">
-        <v>2</v>
-      </c>
-      <c r="C156" s="5">
-        <v>4.3</v>
+        <v>1</v>
+      </c>
+      <c r="C156" s="6">
+        <v>5</v>
       </c>
       <c r="D156">
         <v>0.13600000000000001</v>
@@ -4247,10 +4250,10 @@
         <v>18</v>
       </c>
       <c r="B157" s="3">
-        <v>2</v>
-      </c>
-      <c r="C157" s="5">
-        <v>2.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C157" s="6">
+        <v>8</v>
       </c>
       <c r="D157">
         <v>0.27100000000000002</v>
@@ -4270,10 +4273,10 @@
         <v>18</v>
       </c>
       <c r="B158" s="3">
-        <v>2</v>
-      </c>
-      <c r="C158" s="5">
-        <v>1.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C158" s="6">
+        <v>10</v>
       </c>
       <c r="D158">
         <v>0.53400000000000003</v>
@@ -4293,10 +4296,10 @@
         <v>18</v>
       </c>
       <c r="B159" s="3">
-        <v>2</v>
-      </c>
-      <c r="C159" s="5">
-        <v>1.8999999999999986</v>
+        <v>1</v>
+      </c>
+      <c r="C159" s="6">
+        <v>12</v>
       </c>
       <c r="D159">
         <v>0.76200000000000001</v>
@@ -4316,10 +4319,10 @@
         <v>18</v>
       </c>
       <c r="B160" s="3">
-        <v>2</v>
-      </c>
-      <c r="C160" s="5">
-        <v>1.8500000000000014</v>
+        <v>1</v>
+      </c>
+      <c r="C160" s="6">
+        <v>14</v>
       </c>
       <c r="D160">
         <v>1.07</v>
@@ -4339,10 +4342,10 @@
         <v>18</v>
       </c>
       <c r="B161" s="3">
-        <v>2</v>
-      </c>
-      <c r="C161" s="5">
-        <v>1.8699999999999992</v>
+        <v>1</v>
+      </c>
+      <c r="C161" s="6">
+        <v>16</v>
       </c>
       <c r="D161">
         <v>1.371</v>
@@ -4362,10 +4365,10 @@
         <v>18</v>
       </c>
       <c r="B162" s="3">
-        <v>2</v>
-      </c>
-      <c r="C162" s="5">
-        <v>4.3</v>
+        <v>1</v>
+      </c>
+      <c r="C162" s="6">
+        <v>5</v>
       </c>
       <c r="D162">
         <v>0.34200000000000003</v>
@@ -4385,10 +4388,10 @@
         <v>18</v>
       </c>
       <c r="B163" s="3">
-        <v>2</v>
-      </c>
-      <c r="C163" s="5">
-        <v>2.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C163" s="6">
+        <v>8</v>
       </c>
       <c r="D163">
         <v>0.95799999999999996</v>
@@ -4408,10 +4411,10 @@
         <v>18</v>
       </c>
       <c r="B164" s="3">
-        <v>2</v>
-      </c>
-      <c r="C164" s="5">
-        <v>1.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C164" s="6">
+        <v>10</v>
       </c>
       <c r="D164">
         <v>1.5049999999999999</v>
@@ -4431,10 +4434,10 @@
         <v>18</v>
       </c>
       <c r="B165" s="3">
-        <v>2</v>
-      </c>
-      <c r="C165" s="5">
-        <v>1.8999999999999986</v>
+        <v>1</v>
+      </c>
+      <c r="C165" s="6">
+        <v>12</v>
       </c>
       <c r="D165">
         <v>1.843</v>
@@ -4454,10 +4457,10 @@
         <v>18</v>
       </c>
       <c r="B166" s="3">
-        <v>2</v>
-      </c>
-      <c r="C166" s="5">
-        <v>1.8500000000000014</v>
+        <v>1</v>
+      </c>
+      <c r="C166" s="6">
+        <v>14</v>
       </c>
       <c r="D166">
         <v>2.294</v>
@@ -4477,10 +4480,10 @@
         <v>18</v>
       </c>
       <c r="B167" s="3">
-        <v>2</v>
-      </c>
-      <c r="C167" s="5">
-        <v>1.8699999999999992</v>
+        <v>1</v>
+      </c>
+      <c r="C167" s="6">
+        <v>16</v>
       </c>
       <c r="D167">
         <v>2.9089999999999998</v>
@@ -4500,10 +4503,10 @@
         <v>18</v>
       </c>
       <c r="B168" s="3">
-        <v>2</v>
-      </c>
-      <c r="C168" s="5">
-        <v>4.3</v>
+        <v>1</v>
+      </c>
+      <c r="C168" s="6">
+        <v>5</v>
       </c>
       <c r="D168">
         <v>0.14899999999999999</v>
@@ -4523,10 +4526,10 @@
         <v>18</v>
       </c>
       <c r="B169" s="3">
-        <v>2</v>
-      </c>
-      <c r="C169" s="5">
-        <v>2.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C169" s="6">
+        <v>8</v>
       </c>
       <c r="D169">
         <v>0.28299999999999997</v>
@@ -4546,10 +4549,10 @@
         <v>18</v>
       </c>
       <c r="B170" s="3">
-        <v>2</v>
-      </c>
-      <c r="C170" s="5">
-        <v>1.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C170" s="6">
+        <v>10</v>
       </c>
       <c r="D170">
         <v>0.53300000000000003</v>
@@ -4569,10 +4572,10 @@
         <v>18</v>
       </c>
       <c r="B171" s="3">
-        <v>2</v>
-      </c>
-      <c r="C171" s="5">
-        <v>1.8999999999999986</v>
+        <v>1</v>
+      </c>
+      <c r="C171" s="6">
+        <v>12</v>
       </c>
       <c r="D171">
         <v>0.73199999999999998</v>
@@ -4592,10 +4595,10 @@
         <v>18</v>
       </c>
       <c r="B172" s="3">
-        <v>2</v>
-      </c>
-      <c r="C172" s="5">
-        <v>1.8500000000000014</v>
+        <v>1</v>
+      </c>
+      <c r="C172" s="6">
+        <v>14</v>
       </c>
       <c r="D172">
         <v>0.99099999999999999</v>
@@ -4615,10 +4618,10 @@
         <v>18</v>
       </c>
       <c r="B173" s="3">
-        <v>2</v>
-      </c>
-      <c r="C173" s="5">
-        <v>1.8699999999999992</v>
+        <v>1</v>
+      </c>
+      <c r="C173" s="6">
+        <v>16</v>
       </c>
       <c r="D173">
         <v>1.246</v>
@@ -4638,10 +4641,10 @@
         <v>18</v>
       </c>
       <c r="B174" s="3">
-        <v>2</v>
-      </c>
-      <c r="C174" s="5">
-        <v>4.3</v>
+        <v>1</v>
+      </c>
+      <c r="C174" s="6">
+        <v>5</v>
       </c>
       <c r="D174">
         <v>0.34300000000000003</v>
@@ -4661,10 +4664,10 @@
         <v>18</v>
       </c>
       <c r="B175" s="3">
-        <v>2</v>
-      </c>
-      <c r="C175" s="5">
-        <v>2.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C175" s="6">
+        <v>8</v>
       </c>
       <c r="D175">
         <v>0.95799999999999996</v>
@@ -4684,10 +4687,10 @@
         <v>18</v>
       </c>
       <c r="B176" s="3">
-        <v>2</v>
-      </c>
-      <c r="C176" s="5">
-        <v>1.9000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="C176" s="6">
+        <v>10</v>
       </c>
       <c r="D176">
         <v>1.504</v>
@@ -4707,10 +4710,10 @@
         <v>18</v>
       </c>
       <c r="B177" s="3">
-        <v>2</v>
-      </c>
-      <c r="C177" s="5">
-        <v>1.8999999999999986</v>
+        <v>1</v>
+      </c>
+      <c r="C177" s="6">
+        <v>12</v>
       </c>
       <c r="D177">
         <v>1.8420000000000001</v>
@@ -4730,10 +4733,10 @@
         <v>18</v>
       </c>
       <c r="B178" s="3">
-        <v>2</v>
-      </c>
-      <c r="C178" s="5">
-        <v>1.8500000000000014</v>
+        <v>1</v>
+      </c>
+      <c r="C178" s="6">
+        <v>14</v>
       </c>
       <c r="D178">
         <v>2.2930000000000001</v>
@@ -4753,10 +4756,10 @@
         <v>18</v>
       </c>
       <c r="B179" s="3">
-        <v>2</v>
-      </c>
-      <c r="C179" s="5">
-        <v>1.8699999999999992</v>
+        <v>1</v>
+      </c>
+      <c r="C179" s="6">
+        <v>16</v>
       </c>
       <c r="D179">
         <v>2.9079999999999999</v>
@@ -6363,10 +6366,10 @@
         <v>23</v>
       </c>
       <c r="B249" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C249" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D249">
         <v>0.69</v>
@@ -6386,10 +6389,10 @@
         <v>23</v>
       </c>
       <c r="B250" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C250" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D250">
         <v>1.39</v>
@@ -6432,10 +6435,10 @@
         <v>23</v>
       </c>
       <c r="B252" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C252" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D252">
         <v>0.75</v>
@@ -6455,10 +6458,10 @@
         <v>23</v>
       </c>
       <c r="B253" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C253" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D253">
         <v>1.72</v>
@@ -6501,10 +6504,10 @@
         <v>23</v>
       </c>
       <c r="B255" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C255" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D255">
         <v>0.6</v>
@@ -6524,10 +6527,10 @@
         <v>23</v>
       </c>
       <c r="B256" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C256" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D256">
         <v>2.27</v>
@@ -6570,10 +6573,10 @@
         <v>23</v>
       </c>
       <c r="B258" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C258" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D258">
         <v>1.02</v>
@@ -6593,10 +6596,10 @@
         <v>23</v>
       </c>
       <c r="B259" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C259" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D259">
         <v>1.85</v>
@@ -6639,10 +6642,10 @@
         <v>23</v>
       </c>
       <c r="B261" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C261" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D261">
         <v>0.84</v>
@@ -6662,10 +6665,10 @@
         <v>23</v>
       </c>
       <c r="B262" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C262" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D262">
         <v>2.29</v>
@@ -6708,10 +6711,10 @@
         <v>23</v>
       </c>
       <c r="B264" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C264" s="5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D264">
         <v>0.83</v>
@@ -6731,10 +6734,10 @@
         <v>23</v>
       </c>
       <c r="B265" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C265" s="5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D265">
         <v>2.06</v>
@@ -6757,7 +6760,7 @@
         <v>1</v>
       </c>
       <c r="C266" s="5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D266">
         <v>0.20699999999999999</v>
@@ -6780,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="C267" s="5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D267">
         <v>9.4E-2</v>
@@ -6803,7 +6806,7 @@
         <v>1</v>
       </c>
       <c r="C268" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D268">
         <v>0.29799999999999999</v>
@@ -6826,7 +6829,7 @@
         <v>1</v>
       </c>
       <c r="C269" s="5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D269">
         <v>0.16600000000000001</v>
@@ -6849,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="C270" s="5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D270">
         <v>7.6999999999999999E-2</v>
@@ -6872,7 +6875,7 @@
         <v>1</v>
       </c>
       <c r="C271" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D271">
         <v>0.249</v>
@@ -6895,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="C272" s="5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D272">
         <v>0.315</v>
@@ -6918,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="C273" s="5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D273">
         <v>0.17</v>
@@ -6941,7 +6944,7 @@
         <v>1</v>
       </c>
       <c r="C274" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D274">
         <v>0.39300000000000002</v>
@@ -6964,7 +6967,7 @@
         <v>1</v>
       </c>
       <c r="C275" s="5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D275">
         <v>0.28899999999999998</v>
@@ -6987,7 +6990,7 @@
         <v>1</v>
       </c>
       <c r="C276" s="5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D276">
         <v>0.16600000000000001</v>
@@ -7010,7 +7013,7 @@
         <v>1</v>
       </c>
       <c r="C277" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D277">
         <v>0.373</v>
@@ -7033,7 +7036,7 @@
         <v>1</v>
       </c>
       <c r="C278" s="5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D278">
         <v>0.221</v>
@@ -7056,7 +7059,7 @@
         <v>1</v>
       </c>
       <c r="C279" s="5">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D279">
         <v>0.155</v>
@@ -7079,7 +7082,7 @@
         <v>1</v>
       </c>
       <c r="C280" s="5">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D280">
         <v>0.33100000000000002</v>

</xml_diff>